<commit_message>
Adding data for the SDG #16.b.1
</commit_message>
<xml_diff>
--- a/NYCindexCodebook.xlsx
+++ b/NYCindexCodebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inmilk306/Documents/GitHub/NYCindex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629A2D1A-D0DA-2244-9FBC-A98DD3602FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18C5A21-C78D-B441-88F9-C8A506838CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="900" windowWidth="27640" windowHeight="15720" xr2:uid="{E79D4226-1801-734F-AC68-2051A7BCBA84}"/>
   </bookViews>
@@ -34,6 +34,59 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Polina Polskaia</author>
+  </authors>
+  <commentList>
+    <comment ref="G24" authorId="0" shapeId="0" xr:uid="{80662FE4-A53D-0849-B341-B9EAAF4B7189}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Polina Polskaia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Check with dashboard 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://app.powerbigov.us/view?r=eyJrIjoiYjg1NWI3YjgtYzkzOS00Nzc0LTkwMDAtNTgzM2I2M2JmYWE1IiwidCI6IjJiOWY1N2ViLTc4ZDEtNDZmYi1iZTgzLWEyYWZkZDdjNjA0MyJ9</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="124">
   <si>
@@ -413,7 +466,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,6 +493,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -813,12 +879,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5348E3-1229-414F-9BA4-BB79CA44B88E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5348E3-1229-414F-9BA4-BB79CA44B88E}">
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R25" sqref="R25"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1392,6 +1458,7 @@
     <hyperlink ref="M24" r:id="rId1" display="https://data.cityofnewyork.us/Public-Safety/NYPD-Hate-Crimes/bqiq-cu78" xr:uid="{3AC0071F-8D70-BB44-A8A5-C1AA090D5BE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>